<commit_message>
Alarms Log & Historical fix query read data & exportExcel
</commit_message>
<xml_diff>
--- a/PressMon.Web/wwwroot/assets/docTemplate/TemplateHistorical.xlsx
+++ b/PressMon.Web/wwwroot/assets/docTemplate/TemplateHistorical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PTM_Plumpang\Pressure Monitoring\Program\PressMon_Plumpang restore\PressMon.Web\wwwroot\assets\docTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PTM_Plumpang\Pressure Monitoring\Program\PressMon_Plumpang\PressMon.Web\wwwroot\assets\docTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51507C44-C293-4453-8690-841CF4124A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048DC5D1-B86A-4CB3-9212-23CA0FFAD359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Tanggal Export:</t>
-  </si>
-  <si>
-    <t>Crew Name      :</t>
   </si>
   <si>
     <t>TERMINAL BBM Plumpang</t>
@@ -55,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,20 +126,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -160,7 +154,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -548,11 +542,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,12 +558,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -577,10 +571,10 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -588,12 +582,12 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -601,12 +595,12 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -622,40 +616,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" t="s">
-        <v>0</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>